<commit_message>
Planning for Part I Complete
</commit_message>
<xml_diff>
--- a/Gannt.xlsx
+++ b/Gannt.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blink\Google Drive\University\Year 2\COMP208\Studioruum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619F27E4-3EB0-4798-911F-296652021F03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE2DD8E-7DC5-4731-AFAD-29121C91DAA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7343B4A2-938C-4C1A-ADB8-EFBE2A50E93C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7343B4A2-938C-4C1A-ADB8-EFBE2A50E93C}"/>
   </bookViews>
   <sheets>
     <sheet name="V1.0" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Week 03</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Meeting 01</t>
   </si>
   <si>
-    <t>WRITE SOME GENERAL PLANNINNG NOTES TOO</t>
-  </si>
-  <si>
     <t>(LJ) Minute 01</t>
   </si>
   <si>
@@ -126,7 +123,37 @@
     <t>(TB) System Requirements</t>
   </si>
   <si>
-    <t>(LJ) Requirements Gannt Chart</t>
+    <t>(LJ) Minute 02</t>
+  </si>
+  <si>
+    <t>Meeting 02</t>
+  </si>
+  <si>
+    <t>(LJ) Global Logical Data Model</t>
+  </si>
+  <si>
+    <t>(DP) Data Dictionary</t>
+  </si>
+  <si>
+    <t>(TB) Logical Table Structure</t>
+  </si>
+  <si>
+    <t>(TB) Physical Table Structure</t>
+  </si>
+  <si>
+    <t>(JC/LS) Interface Design</t>
+  </si>
+  <si>
+    <t>(BC) Transaction Matrix</t>
+  </si>
+  <si>
+    <t>(LJ) Planning / Gannt</t>
+  </si>
+  <si>
+    <t>Meeting 03</t>
+  </si>
+  <si>
+    <t>(LJ) Minute 03</t>
   </si>
 </sst>
 </file>
@@ -180,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -240,11 +267,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +312,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,9 +325,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -292,6 +348,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,7 +360,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -380,10 +445,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>332361</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>4053</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
@@ -404,12 +469,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4029075" y="1333500"/>
-          <a:ext cx="714375" cy="104775"/>
+          <a:off x="4555787" y="1337553"/>
+          <a:ext cx="182394" cy="100722"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 64667"/>
+            <a:gd name="adj1" fmla="val 3333"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -465,6 +530,886 @@
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val 848"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>639042</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>107375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connector: Elbow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB75EECB-956F-4E6B-8C97-F71554B717EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5339197" y="1672072"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>639908</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>121230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>865</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>135082</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Connector: Elbow 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E96D3A93-95E6-44CD-A8F5-4F879498A5D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5340063" y="1876427"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>640775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>130756</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1732</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>144608</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connector: Elbow 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D66383-80AB-4378-BFEF-61C12A2D14E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5340930" y="2076453"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>641639</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>131623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2596</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>145475</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connector: Elbow 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B240C4BA-A160-4EA4-9F08-8D0039A95A75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5341794" y="2648820"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>641641</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>144612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2598</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>158464</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connector: Elbow 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B6B098-672A-4E22-B08D-A95AC6D47313}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5341796" y="2280809"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>642507</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>154138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3464</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>167990</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Connector: Elbow 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F6CFCEB-F1CF-4A12-B200-686D97460490}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5342662" y="2480835"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>642506</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3463</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137683</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connector: Elbow 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F987143-1E86-4769-A144-8E8709F1269B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5342661" y="2831528"/>
+          <a:ext cx="204352" cy="122957"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98728"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>487550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3229</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Elbow 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0B318D9-2A27-4FB4-A0D5-5B5065A2180C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808203" y="3241729"/>
+          <a:ext cx="673854" cy="101546"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 647"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>487553</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100096</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>645</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Connector: Elbow 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7694B082-2756-4AB0-B8A3-F6D0F133047E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808206" y="3338596"/>
+          <a:ext cx="236346" cy="211631"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2185"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>488199</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1291</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138017</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Connector: Elbow 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E89177F-EEDF-49E0-89D1-1A05753F1C15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808852" y="3545886"/>
+          <a:ext cx="236346" cy="211631"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2185"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>488845</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1937</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>148349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Connector: Elbow 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75F3E959-AA9E-4701-AE51-A08B22D2DBAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8809498" y="3746718"/>
+          <a:ext cx="236346" cy="211631"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2185"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>492673</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>124810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>156098</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Connector: Elbow 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD6B905-8AFD-45FF-86B0-DE6F8EF5BE25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="8711227" y="4025997"/>
+          <a:ext cx="412288" cy="229914"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 97799"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>487554</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>109782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>646</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>130913</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Connector: Elbow 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8764BA31-CFDC-4C6E-9A2B-B17806541AD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808207" y="4300782"/>
+          <a:ext cx="236346" cy="211631"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2185"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>488200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>116885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1292</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>138016</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Connector: Elbow 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE25B13-5A44-473C-934F-5742EFA5A2BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808853" y="4498385"/>
+          <a:ext cx="236346" cy="211631"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2185"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>269327</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>111672</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Connector: Elbow 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD3D74B9-DD3D-46F9-8E9E-24A593816F6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11167241" y="4007069"/>
+          <a:ext cx="670035" cy="105103"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1961"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>487550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>3229</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Connector: Elbow 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C41DA77-160F-4EDC-A02B-F0AF3676222B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8793350" y="3241729"/>
+          <a:ext cx="674500" cy="101546"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 647"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -776,7 +1721,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -788,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45759C08-C944-4274-8501-6D52E1634B71}">
-  <dimension ref="B2:DB16"/>
+  <dimension ref="B2:DB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,148 +1772,152 @@
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="13" width="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="15" max="35" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
+    <col min="26" max="35" width="7" bestFit="1" customWidth="1"/>
     <col min="36" max="66" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="67" max="96" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="97" max="106" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9" t="s">
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9" t="s">
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9" t="s">
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9" t="s">
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6"/>
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="6"/>
+      <c r="AR2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9" t="s">
+      <c r="AS2" s="6"/>
+      <c r="AT2" s="6"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="6"/>
+      <c r="AX2" s="6"/>
+      <c r="AY2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9" t="s">
+      <c r="AZ2" s="6"/>
+      <c r="BA2" s="6"/>
+      <c r="BB2" s="6"/>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="6"/>
+      <c r="BE2" s="6"/>
+      <c r="BF2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9" t="s">
+      <c r="BG2" s="6"/>
+      <c r="BH2" s="6"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="6"/>
+      <c r="BK2" s="6"/>
+      <c r="BL2" s="6"/>
+      <c r="BM2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="BN2" s="9"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="9"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
-      <c r="BS2" s="9"/>
-      <c r="BT2" s="9" t="s">
+      <c r="BN2" s="6"/>
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="6"/>
+      <c r="BQ2" s="6"/>
+      <c r="BR2" s="6"/>
+      <c r="BS2" s="6"/>
+      <c r="BT2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="9"/>
-      <c r="BW2" s="9"/>
-      <c r="BX2" s="9"/>
-      <c r="BY2" s="9"/>
-      <c r="BZ2" s="9"/>
-      <c r="CA2" s="9" t="s">
+      <c r="BU2" s="6"/>
+      <c r="BV2" s="6"/>
+      <c r="BW2" s="6"/>
+      <c r="BX2" s="6"/>
+      <c r="BY2" s="6"/>
+      <c r="BZ2" s="6"/>
+      <c r="CA2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="CB2" s="9"/>
-      <c r="CC2" s="9"/>
-      <c r="CD2" s="9"/>
-      <c r="CE2" s="9"/>
-      <c r="CF2" s="9"/>
-      <c r="CG2" s="9"/>
-      <c r="CH2" s="10" t="s">
+      <c r="CB2" s="6"/>
+      <c r="CC2" s="6"/>
+      <c r="CD2" s="6"/>
+      <c r="CE2" s="6"/>
+      <c r="CF2" s="6"/>
+      <c r="CG2" s="6"/>
+      <c r="CH2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CI2" s="11"/>
-      <c r="CJ2" s="11"/>
-      <c r="CK2" s="11"/>
-      <c r="CL2" s="11"/>
-      <c r="CM2" s="11"/>
-      <c r="CN2" s="12"/>
-      <c r="CO2" s="9" t="s">
+      <c r="CI2" s="12"/>
+      <c r="CJ2" s="12"/>
+      <c r="CK2" s="12"/>
+      <c r="CL2" s="12"/>
+      <c r="CM2" s="12"/>
+      <c r="CN2" s="13"/>
+      <c r="CO2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="CP2" s="9"/>
-      <c r="CQ2" s="9"/>
-      <c r="CR2" s="9"/>
-      <c r="CS2" s="9"/>
-      <c r="CT2" s="9"/>
-      <c r="CU2" s="9"/>
-      <c r="CV2" s="9" t="s">
+      <c r="CP2" s="6"/>
+      <c r="CQ2" s="6"/>
+      <c r="CR2" s="6"/>
+      <c r="CS2" s="6"/>
+      <c r="CT2" s="6"/>
+      <c r="CU2" s="6"/>
+      <c r="CV2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="CW2" s="9"/>
-      <c r="CX2" s="9"/>
-      <c r="CY2" s="9"/>
-      <c r="CZ2" s="9"/>
-      <c r="DA2" s="9"/>
-      <c r="DB2" s="9"/>
+      <c r="CW2" s="6"/>
+      <c r="CX2" s="6"/>
+      <c r="CY2" s="6"/>
+      <c r="CZ2" s="6"/>
+      <c r="DA2" s="6"/>
+      <c r="DB2" s="6"/>
     </row>
     <row r="3" spans="2:106" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
@@ -1264,121 +2237,121 @@
       </c>
     </row>
     <row r="4" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="14" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="13" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="20" t="s">
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4" s="20"/>
-      <c r="AO4" s="20"/>
-      <c r="AP4" s="20"/>
-      <c r="AQ4" s="20"/>
-      <c r="AR4" s="20"/>
-      <c r="AS4" s="20"/>
-      <c r="AT4" s="20"/>
-      <c r="AU4" s="20"/>
-      <c r="AV4" s="20"/>
-      <c r="AW4" s="20"/>
-      <c r="AX4" s="20"/>
-      <c r="AY4" s="20"/>
-      <c r="AZ4" s="20"/>
-      <c r="BA4" s="20"/>
-      <c r="BB4" s="20"/>
-      <c r="BC4" s="20"/>
-      <c r="BD4" s="20"/>
-      <c r="BE4" s="20"/>
-      <c r="BF4" s="20"/>
-      <c r="BG4" s="20"/>
-      <c r="BH4" s="20"/>
-      <c r="BI4" s="20"/>
-      <c r="BJ4" s="20"/>
-      <c r="BK4" s="20"/>
-      <c r="BL4" s="20"/>
-      <c r="BM4" s="20"/>
-      <c r="BN4" s="20"/>
-      <c r="BO4" s="20"/>
-      <c r="BP4" s="20"/>
-      <c r="BQ4" s="20"/>
-      <c r="BR4" s="20"/>
-      <c r="BS4" s="20"/>
-      <c r="BT4" s="20"/>
-      <c r="BU4" s="20"/>
-      <c r="BV4" s="20"/>
-      <c r="BW4" s="20"/>
-      <c r="BX4" s="20"/>
-      <c r="BY4" s="20"/>
-      <c r="BZ4" s="20"/>
-      <c r="CA4" s="20"/>
-      <c r="CB4" s="20"/>
-      <c r="CC4" s="20"/>
-      <c r="CD4" s="20"/>
-      <c r="CE4" s="20"/>
-      <c r="CF4" s="20"/>
-      <c r="CG4" s="20"/>
-      <c r="CH4" s="20"/>
-      <c r="CI4" s="20"/>
-      <c r="CJ4" s="20"/>
-      <c r="CK4" s="20"/>
-      <c r="CL4" s="20"/>
-      <c r="CM4" s="5" t="s">
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="18"/>
+      <c r="AP4" s="18"/>
+      <c r="AQ4" s="18"/>
+      <c r="AR4" s="18"/>
+      <c r="AS4" s="18"/>
+      <c r="AT4" s="18"/>
+      <c r="AU4" s="18"/>
+      <c r="AV4" s="18"/>
+      <c r="AW4" s="18"/>
+      <c r="AX4" s="18"/>
+      <c r="AY4" s="18"/>
+      <c r="AZ4" s="18"/>
+      <c r="BA4" s="18"/>
+      <c r="BB4" s="18"/>
+      <c r="BC4" s="18"/>
+      <c r="BD4" s="18"/>
+      <c r="BE4" s="18"/>
+      <c r="BF4" s="18"/>
+      <c r="BG4" s="18"/>
+      <c r="BH4" s="18"/>
+      <c r="BI4" s="18"/>
+      <c r="BJ4" s="18"/>
+      <c r="BK4" s="18"/>
+      <c r="BL4" s="18"/>
+      <c r="BM4" s="18"/>
+      <c r="BN4" s="18"/>
+      <c r="BO4" s="18"/>
+      <c r="BP4" s="18"/>
+      <c r="BQ4" s="18"/>
+      <c r="BR4" s="18"/>
+      <c r="BS4" s="18"/>
+      <c r="BT4" s="18"/>
+      <c r="BU4" s="18"/>
+      <c r="BV4" s="18"/>
+      <c r="BW4" s="18"/>
+      <c r="BX4" s="18"/>
+      <c r="BY4" s="18"/>
+      <c r="BZ4" s="18"/>
+      <c r="CA4" s="18"/>
+      <c r="CB4" s="18"/>
+      <c r="CC4" s="18"/>
+      <c r="CD4" s="18"/>
+      <c r="CE4" s="18"/>
+      <c r="CF4" s="18"/>
+      <c r="CG4" s="18"/>
+      <c r="CH4" s="18"/>
+      <c r="CI4" s="18"/>
+      <c r="CJ4" s="18"/>
+      <c r="CK4" s="18"/>
+      <c r="CL4" s="18"/>
+      <c r="CM4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="CN4" s="5"/>
-      <c r="CO4" s="5"/>
-      <c r="CP4" s="5"/>
-      <c r="CQ4" s="5"/>
-      <c r="CR4" s="5"/>
-      <c r="CS4" s="5"/>
-      <c r="CT4" s="5"/>
-      <c r="CU4" s="5"/>
-      <c r="CV4" s="5"/>
-      <c r="CW4" s="5"/>
-      <c r="CX4" s="5"/>
-      <c r="CY4" s="5"/>
-      <c r="CZ4" s="5"/>
-      <c r="DA4" s="5"/>
-      <c r="DB4" s="5"/>
+      <c r="CN4" s="7"/>
+      <c r="CO4" s="7"/>
+      <c r="CP4" s="7"/>
+      <c r="CQ4" s="7"/>
+      <c r="CR4" s="7"/>
+      <c r="CS4" s="7"/>
+      <c r="CT4" s="7"/>
+      <c r="CU4" s="7"/>
+      <c r="CV4" s="7"/>
+      <c r="CW4" s="7"/>
+      <c r="CX4" s="7"/>
+      <c r="CY4" s="7"/>
+      <c r="CZ4" s="7"/>
+      <c r="DA4" s="7"/>
+      <c r="DB4" s="7"/>
     </row>
     <row r="5" spans="2:106" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -1488,14 +2461,14 @@
       <c r="DB5" s="1"/>
     </row>
     <row r="6" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1604,10 +2577,10 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="4"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1711,91 +2684,230 @@
       </c>
     </row>
     <row r="9" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="M9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="5"/>
+      <c r="M9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="L10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="L10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="L11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+      <c r="L11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="L12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="L12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="L14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="L14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="L15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="8"/>
+      <c r="L15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:106" x14ac:dyDescent="0.25">
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="R17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
+    </row>
+    <row r="18" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="T18" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="U18" s="22"/>
+    </row>
+    <row r="19" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+    </row>
+    <row r="20" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+    </row>
+    <row r="21" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+    </row>
+    <row r="22" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+    </row>
+    <row r="23" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+    </row>
+    <row r="24" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+    </row>
+    <row r="25" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="S25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+    </row>
+    <row r="26" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="Y26" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="18:30" x14ac:dyDescent="0.25">
+      <c r="AA27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB27" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="P2:V2"/>
-    <mergeCell ref="W2:AC2"/>
-    <mergeCell ref="AD2:AJ2"/>
+  <mergeCells count="40">
+    <mergeCell ref="AA27:AB27"/>
+    <mergeCell ref="S22:X22"/>
+    <mergeCell ref="Y22:AD22"/>
+    <mergeCell ref="S23:AD23"/>
+    <mergeCell ref="S24:AD24"/>
+    <mergeCell ref="S25:AD25"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="S21:X21"/>
+    <mergeCell ref="S19:AD19"/>
+    <mergeCell ref="S20:AD20"/>
+    <mergeCell ref="L13:Q13"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="CM4:DB4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L10:Q10"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="B4:H4"/>
     <mergeCell ref="L16:Q16"/>
     <mergeCell ref="L15:Q15"/>
     <mergeCell ref="CV2:DB2"/>
@@ -1812,15 +2924,11 @@
     <mergeCell ref="CA2:CG2"/>
     <mergeCell ref="AK2:AQ2"/>
     <mergeCell ref="L14:Q14"/>
-    <mergeCell ref="L13:Q13"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="CM4:DB4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="L10:Q10"/>
-    <mergeCell ref="L11:Q11"/>
-    <mergeCell ref="L12:Q12"/>
-    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="P2:V2"/>
+    <mergeCell ref="W2:AC2"/>
+    <mergeCell ref="AD2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>